<commit_message>
database & requests successfully added
</commit_message>
<xml_diff>
--- a/database/URLS.xlsx
+++ b/database/URLS.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="15">
   <si>
     <t>https://en.zalando.de/men-clothing-shirts/</t>
   </si>
@@ -395,7 +395,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:A15"/>
+  <dimension ref="A1:A30"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -476,6 +476,81 @@
         <v>14</v>
       </c>
     </row>
+    <row r="16">
+      <c r="A16" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="s">
+        <v>14</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>

</xml_diff>